<commit_message>
Fazendo a função de atualizar falores do preço do dolar no banco
</commit_message>
<xml_diff>
--- a/bot-cotacao-dolar/produtos.xlsx
+++ b/bot-cotacao-dolar/produtos.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>68.88</t>
+          <t>68.72</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>25.90</t>
+          <t>25.84</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>95.33</t>
+          <t>95.11</t>
         </is>
       </c>
     </row>

</xml_diff>